<commit_message>
neue Grafiken und ein wenig Korrekturen
</commit_message>
<xml_diff>
--- a/Thesis/BewertungsDaten/Genauigkeit/CPD_Rotation/RotationTest10MitDiagramm.xlsx
+++ b/Thesis/BewertungsDaten/Genauigkeit/CPD_Rotation/RotationTest10MitDiagramm.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Repositorys\Thesis\Thesis\BewertungsDaten\Genauigkeit\CPD_Rotation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jknopp\Desktop\Repositorys\Thesis\Thesis\BewertungsDaten\Genauigkeit\CPD_Rotation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{468E52E9-F17F-40E8-937A-D87665E633C9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-1590" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-1590" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="RotationTest10" sheetId="1" r:id="rId1"/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -611,6 +610,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -929,6 +929,7 @@
         <c:axId val="446378256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="350"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -972,6 +973,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1089,6 +1091,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1169,6 +1172,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -1176,7 +1180,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2104,11 +2107,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView tabSelected="1" topLeftCell="E7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>